<commit_message>
update readme and data sprint 1-2
</commit_message>
<xml_diff>
--- a/Data/bienban_sprint1/sprint1.xlsx
+++ b/Data/bienban_sprint1/sprint1.xlsx
@@ -198,7 +198,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -245,6 +245,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -524,7 +531,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1060,7 +1067,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>